<commit_message>
Se sube json de ejemplo de primer evento
</commit_message>
<xml_diff>
--- a/docs/StructureDefinition-PractitioneRolerLE.xlsx
+++ b/docs/StructureDefinition-PractitioneRolerLE.xlsx
@@ -36,7 +36,7 @@
     <t>Name</t>
   </si>
   <si>
-    <t>PractitioneRolerLE</t>
+    <t>PractitionerRoleLE</t>
   </si>
   <si>
     <t>Title</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-01-30T23:51:40-03:00</t>
+    <t>2023-01-31T15:14:06-03:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>